<commit_message>
Add invoiceunprocesslit integration api.
</commit_message>
<xml_diff>
--- a/payload/wms connector/invoice/invoice mapping.xlsx
+++ b/payload/wms connector/invoice/invoice mapping.xlsx
@@ -7,20 +7,20 @@
     <workbookView windowWidth="23040" windowHeight="9420"/>
   </bookViews>
   <sheets>
-    <sheet name="Order header" sheetId="4" r:id="rId1"/>
-    <sheet name="orderitem" sheetId="5" r:id="rId2"/>
+    <sheet name="InvoiceHeader" sheetId="4" r:id="rId1"/>
+    <sheet name="InvoiceItems" sheetId="5" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="6" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Order header'!$D$1:$D$29</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">orderitem!#REF!</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">InvoiceHeader!$D$1:$D$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">InvoiceItems!#REF!</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="101">
   <si>
     <t>column type</t>
   </si>
@@ -158,6 +158,12 @@
   </si>
   <si>
     <t xml:space="preserve">        public decimal ShippingCost = 0;</t>
+  </si>
+  <si>
+    <t>ShippingAmount</t>
+  </si>
+  <si>
+    <t>ShippingAmount+ShippingTaxAmount?</t>
   </si>
   <si>
     <t>ShippingCost</t>
@@ -378,13 +384,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -399,7 +398,28 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -408,14 +428,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -445,6 +457,14 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
@@ -469,14 +489,6 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
@@ -484,16 +496,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -507,8 +512,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -535,181 +541,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -810,6 +816,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -824,17 +841,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -843,10 +849,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -855,7 +861,7 @@
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -864,128 +870,128 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1005,9 +1011,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
@@ -1369,8 +1372,8 @@
   <sheetPr/>
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F20" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H29"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -1383,39 +1386,39 @@
     <col min="6" max="6" width="24.7777777777778" style="7" customWidth="1"/>
     <col min="7" max="7" width="40.8888888888889" style="7" customWidth="1"/>
     <col min="8" max="8" width="66.6666666666667" style="7" customWidth="1"/>
-    <col min="9" max="9" width="70.6666666666667" style="8" customWidth="1"/>
+    <col min="9" max="9" width="70.6666666666667" style="7" customWidth="1"/>
     <col min="10" max="10" width="40.3333333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="1" spans="1:9">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9" t="s">
+      <c r="E1" s="8"/>
+      <c r="F1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
     </row>
     <row r="2" customFormat="1" ht="25.2" customHeight="1" spans="1:9">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -1424,7 +1427,7 @@
       <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="G2" s="2" t="str">
@@ -1444,7 +1447,7 @@
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -1474,7 +1477,7 @@
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -1504,7 +1507,7 @@
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -1534,7 +1537,7 @@
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -1564,7 +1567,7 @@
       <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -1594,7 +1597,7 @@
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -1624,7 +1627,7 @@
       <c r="A9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -1656,7 +1659,7 @@
       <c r="A10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -1686,7 +1689,7 @@
       <c r="A11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -1716,13 +1719,15 @@
       <c r="A12" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="2"/>
+      <c r="D12" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="E12" s="2" t="s">
         <v>9</v>
       </c>
@@ -1746,7 +1751,7 @@
       <c r="A13" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -1778,7 +1783,7 @@
       <c r="A14" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -1810,8 +1815,8 @@
       <c r="A15" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>6</v>
+      <c r="B15" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>39</v>
@@ -1831,18 +1836,18 @@
       </c>
       <c r="H15" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{InfoHelper.TableAllies}.ShipDate as '{header}.ShipmentDateUtc',</v>
+        <v>{Helper.TableAllies}.ShipDate as '{header}.ShipmentDateUtc',</v>
       </c>
       <c r="I15" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>{InfoHelper.TableAllies}.ShipDate AS ShipmentDateUtc,</v>
+        <v>{Helper.TableAllies}.ShipDate AS ShipmentDateUtc,</v>
       </c>
     </row>
     <row r="16" ht="37.8" customHeight="1" spans="1:9">
       <c r="A16" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -1872,7 +1877,7 @@
       <c r="A17" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -1902,18 +1907,20 @@
       <c r="A18" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="2"/>
+      <c r="D18" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="E18" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G18" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1921,22 +1928,22 @@
       </c>
       <c r="H18" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{InfoHelper.TableAllies}.ShippingCost as '{header}.ShippingCost',</v>
+        <v>{InfoHelper.TableAllies}.ShippingAmount as '{header}.ShippingCost',</v>
       </c>
       <c r="I18" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>{InfoHelper.TableAllies}.ShippingCost AS ShippingCost,</v>
+        <v>{InfoHelper.TableAllies}.ShippingAmount AS ShippingCost,</v>
       </c>
     </row>
     <row r="19" ht="25.2" customHeight="1" spans="1:9">
       <c r="A19" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B19" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>35</v>
@@ -1945,7 +1952,7 @@
         <v>9</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G19" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1962,20 +1969,20 @@
     </row>
     <row r="20" ht="37.8" customHeight="1" spans="1:9">
       <c r="A20" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G20" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1992,20 +1999,20 @@
     </row>
     <row r="21" ht="37.8" customHeight="1" spans="1:9">
       <c r="A21" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B21" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G21" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2022,22 +2029,22 @@
     </row>
     <row r="22" ht="37.8" customHeight="1" spans="1:9">
       <c r="A22" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B22" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G22" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2054,20 +2061,20 @@
     </row>
     <row r="23" ht="50.4" customHeight="1" spans="1:9">
       <c r="A23" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B23" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="G23" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2084,20 +2091,20 @@
     </row>
     <row r="24" ht="37.8" customHeight="1" spans="1:9">
       <c r="A24" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B24" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G24" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2114,13 +2121,13 @@
     </row>
     <row r="25" ht="37.8" customHeight="1" spans="1:9">
       <c r="A25" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B25" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="10" t="s">
-        <v>64</v>
+      <c r="C25" s="9" t="s">
+        <v>66</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>8</v>
@@ -2129,7 +2136,7 @@
         <v>9</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G25" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2146,20 +2153,20 @@
     </row>
     <row r="26" ht="37.8" customHeight="1" spans="1:9">
       <c r="A26" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B26" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G26" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2176,20 +2183,20 @@
     </row>
     <row r="27" ht="37.8" customHeight="1" spans="1:9">
       <c r="A27" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B27" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G27" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2206,13 +2213,13 @@
     </row>
     <row r="28" ht="25.2" customHeight="1" spans="1:9">
       <c r="A28" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B28" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="10" t="s">
-        <v>72</v>
+      <c r="C28" s="9" t="s">
+        <v>74</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>8</v>
@@ -2221,7 +2228,7 @@
         <v>9</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G28" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2238,13 +2245,13 @@
     </row>
     <row r="29" ht="37.8" customHeight="1" spans="1:9">
       <c r="A29" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B29" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B29" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C29" s="10" t="s">
-        <v>74</v>
+      <c r="C29" s="9" t="s">
+        <v>76</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>8</v>
@@ -2253,7 +2260,7 @@
         <v>9</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G29" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2318,22 +2325,22 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" ht="60" spans="1:8">
+    <row r="2" ht="37.8" spans="1:8">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G2" s="2" t="str">
         <f t="shared" ref="G2:G29" si="0">REPLACE(E2,4,1,F2)</f>
@@ -2344,21 +2351,21 @@
         <v>{ItemHelper.TableAllies}.Seq AS OrderInvoiceLineNum,</v>
       </c>
     </row>
-    <row r="3" ht="45" spans="1:8">
+    <row r="3" ht="25.2" spans="1:8">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>12</v>
@@ -2372,21 +2379,21 @@
         <v>{ItemHelper.TableAllies}.DatabaseNum AS DatabaseNum,</v>
       </c>
     </row>
-    <row r="4" ht="60" spans="1:8">
+    <row r="4" ht="37.8" spans="1:8">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>14</v>
@@ -2400,21 +2407,21 @@
         <v>{ItemHelper.TableAllies}.MasterAccountNum AS MasterAccountNum,</v>
       </c>
     </row>
-    <row r="5" ht="45" spans="1:8">
+    <row r="5" ht="15" spans="1:8">
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>16</v>
@@ -2428,21 +2435,21 @@
         <v>{ItemHelper.TableAllies}.ProfileNum AS ProfileNum,</v>
       </c>
     </row>
-    <row r="6" ht="45" spans="1:8">
+    <row r="6" ht="15" spans="1:8">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>18</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>18</v>
@@ -2456,21 +2463,21 @@
         <v>{ItemHelper.TableAllies}.ChannelNum AS ChannelNum,</v>
       </c>
     </row>
-    <row r="7" ht="60" spans="1:8">
+    <row r="7" ht="37.8" spans="1:8">
       <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>20</v>
@@ -2484,24 +2491,24 @@
         <v>{ItemHelper.TableAllies}.ChannelAccountNum AS ChannelAccountNum,</v>
       </c>
     </row>
-    <row r="8" ht="45" spans="1:8">
+    <row r="8" ht="37.8" spans="1:8">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>35</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G8" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2512,24 +2519,24 @@
         <v>{ItemHelper.TableAllies}.OrderShipmentItemNum AS OrderShipmentItemNum,</v>
       </c>
     </row>
-    <row r="9" ht="45" spans="1:8">
+    <row r="9" ht="37.8" spans="1:8">
       <c r="A9" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G9" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2540,24 +2547,24 @@
         <v>{ItemHelper.TableAllies}.CentralOrderLineNum AS CentralOrderLineNum,</v>
       </c>
     </row>
-    <row r="10" ht="60" spans="1:8">
+    <row r="10" ht="37.8" spans="1:8">
       <c r="A10" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G10" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2568,22 +2575,22 @@
         <v>{ItemHelper.TableAllies}.OrderDCAssignmentLineNum AS OrderDCAssignmentLineNum,</v>
       </c>
     </row>
-    <row r="11" ht="30" spans="1:8">
+    <row r="11" ht="25.2" spans="1:8">
       <c r="A11" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G11" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2594,24 +2601,24 @@
         <v>{ItemHelper.TableAllies}.SKU AS SKU,</v>
       </c>
     </row>
-    <row r="12" ht="45" spans="1:8">
+    <row r="12" ht="25.2" spans="1:8">
       <c r="A12" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G12" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2622,22 +2629,22 @@
         <v>{ItemHelper.TableAllies}.ChannelItemID AS ChannelItemID,</v>
       </c>
     </row>
-    <row r="13" ht="45" spans="1:8">
+    <row r="13" ht="25.2" spans="1:8">
       <c r="A13" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="G13" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2648,22 +2655,22 @@
         <v>{ItemHelper.TableAllies}.ShipQty AS ShippedQty,</v>
       </c>
     </row>
-    <row r="14" ht="45" spans="1:8">
+    <row r="14" ht="25.2" spans="1:8">
       <c r="A14" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="G14" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2674,22 +2681,22 @@
         <v>{ItemHelper.TableAllies}.DiscountPrice AS UnitPrice,</v>
       </c>
     </row>
-    <row r="15" ht="45" spans="1:8">
+    <row r="15" ht="25.2" spans="1:8">
       <c r="A15" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="G15" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2700,22 +2707,22 @@
         <v>{ItemHelper.TableAllies}.ExtAmount AS LineItemAmount,</v>
       </c>
     </row>
-    <row r="16" ht="45" spans="1:8">
+    <row r="16" ht="25.2" spans="1:8">
       <c r="A16" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G16" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2726,22 +2733,22 @@
         <v>{ItemHelper.TableAllies}.TaxAmount AS LineTaxAmount,</v>
       </c>
     </row>
-    <row r="17" ht="45" spans="1:8">
+    <row r="17" ht="37.8" spans="1:8">
       <c r="A17" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="G17" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2752,132 +2759,132 @@
         <v>{ItemHelper.TableAllies}.ChargeAndAllowanceAmount AS LineHandlingFee,</v>
       </c>
     </row>
-    <row r="18" ht="45" spans="1:8">
+    <row r="18" ht="37.8" spans="1:8">
       <c r="A18" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="G18" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>as LineDiscountAmount</v>
+      </c>
+      <c r="H18" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>{ItemHelper.TableAllies}.DiscountAmount AS LineDiscountAmount,</v>
+      </c>
+    </row>
+    <row r="19" ht="25.2" spans="1:8">
+      <c r="A19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="F18" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="G18" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>as LineDiscountAmount</v>
-      </c>
-      <c r="H18" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>{ItemHelper.TableAllies}.DiscountAmount AS LineDiscountAmount,</v>
-      </c>
-    </row>
-    <row r="19" ht="45" spans="1:8">
-      <c r="A19" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>75</v>
-      </c>
       <c r="C19" s="4" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G19" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>as LineAmount</v>
+      </c>
+      <c r="H19" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>{ItemHelper.TableAllies}.ItemTotalAmount AS LineAmount,</v>
+      </c>
+    </row>
+    <row r="20" ht="37.8" spans="1:8">
+      <c r="A20" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="F19" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="G19" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>as LineAmount</v>
-      </c>
-      <c r="H19" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>{ItemHelper.TableAllies}.ItemTotalAmount AS LineAmount,</v>
-      </c>
-    </row>
-    <row r="20" ht="60" spans="1:8">
-      <c r="A20" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>75</v>
-      </c>
       <c r="C20" s="4" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E20" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G20" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>as DBChannelOrderLineRowID</v>
+      </c>
+      <c r="H20" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>{ItemHelper.TableAllies}.DBChannelOrderLineRowID AS DBChannelOrderLineRowID,</v>
+      </c>
+    </row>
+    <row r="21" ht="25.2" spans="1:8">
+      <c r="A21" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="F20" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="G20" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>as DBChannelOrderLineRowID</v>
-      </c>
-      <c r="H20" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>{ItemHelper.TableAllies}.DBChannelOrderLineRowID AS DBChannelOrderLineRowID,</v>
-      </c>
-    </row>
-    <row r="21" ht="45" spans="1:8">
-      <c r="A21" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>75</v>
-      </c>
       <c r="C21" s="4" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E21" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G21" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>as ItemStatus</v>
+      </c>
+      <c r="H21" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>{ItemHelper.TableAllies}.ItemStatus AS ItemStatus,</v>
+      </c>
+    </row>
+    <row r="22" ht="25.2" spans="1:8">
+      <c r="A22" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="F21" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="G21" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>as ItemStatus</v>
-      </c>
-      <c r="H21" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>{ItemHelper.TableAllies}.ItemStatus AS ItemStatus,</v>
-      </c>
-    </row>
-    <row r="22" ht="45" spans="1:8">
-      <c r="A22" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>75</v>
-      </c>
       <c r="C22" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G22" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2907,7 +2914,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -2937,77 +2944,77 @@
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change po receive logic
</commit_message>
<xml_diff>
--- a/payload/wms connector/invoice/invoice mapping.xlsx
+++ b/payload/wms connector/invoice/invoice mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9420"/>
+    <workbookView windowWidth="22368" windowHeight="9420"/>
   </bookViews>
   <sheets>
     <sheet name="InvoiceHeader" sheetId="4" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="101">
   <si>
     <t>column type</t>
   </si>
@@ -95,9 +95,6 @@
   </si>
   <si>
     <t>InvoiceDate</t>
-  </si>
-  <si>
-    <t>conver to utc date</t>
   </si>
   <si>
     <t>InvoiceDateUtc</t>
@@ -333,10 +330,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -379,31 +376,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -416,30 +391,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -456,7 +407,38 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -471,14 +453,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -500,14 +483,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="宋体"/>
@@ -517,13 +492,35 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -538,109 +535,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -652,73 +721,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -747,17 +750,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -794,35 +802,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
@@ -844,6 +823,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -852,149 +855,149 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1023,6 +1026,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1375,8 +1384,8 @@
   <sheetPr/>
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C18" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" topLeftCell="C14" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -1387,9 +1396,9 @@
     <col min="4" max="4" width="27.5555555555556" style="7" customWidth="1"/>
     <col min="5" max="5" width="23.1111111111111" style="7" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="24.6666666666667" style="7" customWidth="1"/>
-    <col min="7" max="7" width="40.8888888888889" style="7" customWidth="1"/>
-    <col min="8" max="8" width="66.6666666666667" style="7" customWidth="1"/>
-    <col min="9" max="9" width="1.66666666666667" style="7" customWidth="1"/>
+    <col min="7" max="7" width="40.8888888888889" style="7" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="66.6666666666667" style="7" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="1.66666666666667" style="7" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="46.3333333333333" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1636,14 +1645,12 @@
       <c r="C9" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="9" t="s">
-        <v>25</v>
-      </c>
+      <c r="D9" s="9"/>
       <c r="E9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G9" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1660,20 +1667,20 @@
     </row>
     <row r="10" ht="25.2" customHeight="1" spans="1:9">
       <c r="A10" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G10" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1690,20 +1697,20 @@
     </row>
     <row r="11" ht="37.8" customHeight="1" spans="1:9">
       <c r="A11" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G11" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1720,22 +1727,20 @@
     </row>
     <row r="12" ht="25.2" customHeight="1" spans="1:9">
       <c r="A12" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>8</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G12" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1752,20 +1757,20 @@
     </row>
     <row r="13" customHeight="1" spans="1:9">
       <c r="A13" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G13" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1782,22 +1787,22 @@
     </row>
     <row r="14" ht="37.8" customHeight="1" spans="1:9">
       <c r="A14" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G14" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1814,22 +1819,20 @@
     </row>
     <row r="15" ht="37.8" customHeight="1" spans="1:9">
       <c r="A15" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>25</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="D15" s="10"/>
       <c r="E15" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G15" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1846,20 +1849,20 @@
     </row>
     <row r="16" ht="37.8" customHeight="1" spans="1:9">
       <c r="A16" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G16" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1876,20 +1879,20 @@
     </row>
     <row r="17" ht="37.8" customHeight="1" spans="1:9">
       <c r="A17" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G17" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1906,22 +1909,22 @@
     </row>
     <row r="18" ht="25.2" customHeight="1" spans="1:9">
       <c r="A18" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="9" t="s">
         <v>46</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>47</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G18" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1938,22 +1941,22 @@
     </row>
     <row r="19" ht="25.2" customHeight="1" spans="1:9">
       <c r="A19" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>37</v>
+        <v>49</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>36</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G19" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1970,20 +1973,20 @@
     </row>
     <row r="20" ht="37.8" customHeight="1" spans="1:9">
       <c r="A20" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G20" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2000,20 +2003,20 @@
     </row>
     <row r="21" ht="37.8" customHeight="1" spans="1:9">
       <c r="A21" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G21" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2030,22 +2033,22 @@
     </row>
     <row r="22" ht="37.8" customHeight="1" spans="1:9">
       <c r="A22" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>57</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G22" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2062,20 +2065,20 @@
     </row>
     <row r="23" ht="50.4" customHeight="1" spans="1:9">
       <c r="A23" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G23" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2092,20 +2095,20 @@
     </row>
     <row r="24" ht="37.8" customHeight="1" spans="1:9">
       <c r="A24" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G24" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2122,13 +2125,13 @@
     </row>
     <row r="25" ht="37.8" customHeight="1" spans="1:9">
       <c r="A25" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>8</v>
@@ -2137,7 +2140,7 @@
         <v>9</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G25" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2154,20 +2157,20 @@
     </row>
     <row r="26" ht="37.8" customHeight="1" spans="1:9">
       <c r="A26" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G26" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2184,20 +2187,20 @@
     </row>
     <row r="27" ht="37.8" customHeight="1" spans="1:9">
       <c r="A27" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G27" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2214,13 +2217,13 @@
     </row>
     <row r="28" ht="25.2" customHeight="1" spans="1:9">
       <c r="A28" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>8</v>
@@ -2229,7 +2232,7 @@
         <v>9</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G28" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2246,20 +2249,20 @@
     </row>
     <row r="29" ht="37.8" customHeight="1" spans="1:9">
       <c r="A29" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G29" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2329,17 +2332,17 @@
         <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>77</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>78</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>79</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>80</v>
       </c>
       <c r="G2" s="2" t="str">
         <f t="shared" ref="G2:G29" si="0">REPLACE(E2,4,1,F2)</f>
@@ -2355,16 +2358,16 @@
         <v>10</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>12</v>
@@ -2383,16 +2386,16 @@
         <v>13</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>14</v>
@@ -2411,16 +2414,16 @@
         <v>15</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>16</v>
@@ -2439,16 +2442,16 @@
         <v>17</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>18</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>18</v>
@@ -2467,16 +2470,16 @@
         <v>19</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>20</v>
@@ -2495,19 +2498,19 @@
         <v>21</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G8" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2523,19 +2526,19 @@
         <v>23</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>84</v>
-      </c>
       <c r="E9" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G9" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2548,22 +2551,22 @@
     </row>
     <row r="10" ht="37.8" spans="1:8">
       <c r="A10" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>84</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>85</v>
       </c>
       <c r="G10" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2576,20 +2579,20 @@
     </row>
     <row r="11" ht="25.2" spans="1:8">
       <c r="A11" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G11" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2602,22 +2605,22 @@
     </row>
     <row r="12" ht="25.2" spans="1:8">
       <c r="A12" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G12" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2630,20 +2633,20 @@
     </row>
     <row r="13" ht="25.2" spans="1:8">
       <c r="A13" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G13" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2656,20 +2659,20 @@
     </row>
     <row r="14" ht="25.2" spans="1:8">
       <c r="A14" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G14" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2682,20 +2685,20 @@
     </row>
     <row r="15" ht="25.2" spans="1:8">
       <c r="A15" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G15" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2708,20 +2711,20 @@
     </row>
     <row r="16" ht="25.2" spans="1:8">
       <c r="A16" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G16" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2734,20 +2737,20 @@
     </row>
     <row r="17" ht="37.8" spans="1:8">
       <c r="A17" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G17" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2760,20 +2763,20 @@
     </row>
     <row r="18" ht="37.8" spans="1:8">
       <c r="A18" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G18" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2786,20 +2789,20 @@
     </row>
     <row r="19" ht="25.2" spans="1:8">
       <c r="A19" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G19" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2812,22 +2815,22 @@
     </row>
     <row r="20" ht="37.8" spans="1:8">
       <c r="A20" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G20" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2840,20 +2843,20 @@
     </row>
     <row r="21" ht="25.2" spans="1:8">
       <c r="A21" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G21" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2866,20 +2869,20 @@
     </row>
     <row r="22" ht="25.2" spans="1:8">
       <c r="A22" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G22" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2909,7 +2912,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -2939,77 +2942,77 @@
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>